<commit_message>
Lab on Anova statistical analysis
</commit_message>
<xml_diff>
--- a/files_for_lab/anova_lab_data.xlsx
+++ b/files_for_lab/anova_lab_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/himanshuaggarwal/data/01-lesson_plans/07-unit_adv_stats_feature_selecftion_Trees_ensemble_methods/7.05_/lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annakharchenkova/Desktop/Data Sc/Week_7/Day_33_ANOVA/lab-inferential-statistics-anova/files_for_lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BCEDA-F489-CF4E-91D8-0E2205FE340A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39D48F8-A2C9-C44A-BE80-71FBA27D9F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2300" windowWidth="21900" windowHeight="12940" xr2:uid="{49703896-377D-AA4B-83EF-96E6D3254657}"/>
+    <workbookView xWindow="7680" yWindow="2100" windowWidth="21900" windowHeight="12940" xr2:uid="{49703896-377D-AA4B-83EF-96E6D3254657}"/>
   </bookViews>
   <sheets>
     <sheet name="data_collected" sheetId="2" r:id="rId1"/>
@@ -90,10 +90,10 @@
     <t>200 W</t>
   </si>
   <si>
-    <t>Etching Rate</t>
-  </si>
-  <si>
     <t>&lt;0.0001</t>
+  </si>
+  <si>
+    <t>Etching_Rate</t>
   </si>
 </sst>
 </file>
@@ -492,9 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7DA315-ECA9-A947-8813-9D781649E28B}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -503,10 +501,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -695,7 +693,7 @@
         <v>35.777142857142856</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.2">

</xml_diff>